<commit_message>
add context to fixture file, introduce mechanics to us multiple possible locators to access elements
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F0B23F-AB41-4B7A-9870-084C2E72B403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D8648-69EC-46EC-A531-54726583B5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2775" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3045" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -121,6 +121,21 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>calss_name</t>
+  </si>
+  <si>
+    <t>css selector</t>
+  </si>
+  <si>
+    <t>css_selector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpatch </t>
+  </si>
+  <si>
+    <t>collor filters</t>
   </si>
 </sst>
 </file>
@@ -136,12 +151,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,8 +177,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,118 +504,165 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
+      <c r="A8" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D15" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test data is now coming from test record from excel file
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2D8648-69EC-46EC-A531-54726583B5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCBE510-8014-4D36-93DC-6642FC749B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3045" yWindow="1755" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23784" yWindow="768" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -123,19 +123,19 @@
     <t>White</t>
   </si>
   <si>
-    <t>calss_name</t>
-  </si>
-  <si>
-    <t>css selector</t>
-  </si>
-  <si>
-    <t>css_selector</t>
-  </si>
-  <si>
     <t xml:space="preserve">xpatch </t>
   </si>
   <si>
     <t>collor filters</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>current filter</t>
+  </si>
+  <si>
+    <t>breadcrumb</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +510,7 @@
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -564,22 +564,19 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
+      <c r="A9" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -587,10 +584,10 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -601,7 +598,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
filters work in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCBE510-8014-4D36-93DC-6642FC749B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D7D731-3105-412D-A87C-90A22C95A902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23784" yWindow="768" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="840" windowWidth="27000" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
@@ -75,36 +75,21 @@
     <t>Select:</t>
   </si>
   <si>
-    <t>select Black</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
     <t>//div[contains(@class,'custom-filters category-custom-filters')]//li[1]//a[1]//img[1]</t>
   </si>
   <si>
-    <t>select Gold</t>
-  </si>
-  <si>
     <t>//div[contains(@class,'custom-filters category-custom-filters')]//li[2]//a[1]//img[1]</t>
   </si>
   <si>
-    <t>select Pink</t>
-  </si>
-  <si>
     <t>//div[contains(@class,'custom-filters category-custom-filters')]//li[3]//a[1]//img[1]</t>
   </si>
   <si>
-    <t>select Grey</t>
-  </si>
-  <si>
     <t>//div[contains(@class,'custom-filters category-custom-filters')]//li[4]//a[1]//img[1]</t>
   </si>
   <si>
-    <t>select White</t>
-  </si>
-  <si>
     <t>//div[contains(@class,'custom-filters category-custom-filters')]//li[5]//a[1]//img[1]</t>
   </si>
   <si>
@@ -132,20 +117,105 @@
     <t>example</t>
   </si>
   <si>
-    <t>current filter</t>
-  </si>
-  <si>
     <t>breadcrumb</t>
+  </si>
+  <si>
+    <t>price range filters</t>
+  </si>
+  <si>
+    <t>60-79</t>
+  </si>
+  <si>
+    <t>under 20</t>
+  </si>
+  <si>
+    <t>20-39</t>
+  </si>
+  <si>
+    <t>40-59</t>
+  </si>
+  <si>
+    <t>80-99</t>
+  </si>
+  <si>
+    <t>100-249</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'$100 - $249')]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'Under $20')]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'$20 - $39')]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'$40 - $59')]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'$60 - $79')]</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'accordion-content is-open')]//span[contains(text(),'$80 - $99')]</t>
+  </si>
+  <si>
+    <t>$20-$39</t>
+  </si>
+  <si>
+    <t>under $20</t>
+  </si>
+  <si>
+    <t>$40-$59</t>
+  </si>
+  <si>
+    <t>$60-$79</t>
+  </si>
+  <si>
+    <t>$80-$99</t>
+  </si>
+  <si>
+    <t>$100-$249</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,9 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,17 +533,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="76.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -507,10 +580,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -565,102 +638,191 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>33</v>
+      <c r="A9" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>31</v>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: plp page and filters, product selection, pdp_page in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D7D731-3105-412D-A87C-90A22C95A902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14C2C1D-0140-4412-B18C-3882C312C2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="840" windowWidth="27000" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="840" windowWidth="27000" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
+    <sheet name="PDP_Page" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -175,6 +176,27 @@
   </si>
   <si>
     <t>$100-$249</t>
+  </si>
+  <si>
+    <t>product_info</t>
+  </si>
+  <si>
+    <t>AddProductToCartFormProductSummary_productSummary_row__3pIGN</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>otCSfuRyXDDgPcWMS82WHWpQ</t>
+  </si>
+  <si>
+    <t>pt-3.5</t>
+  </si>
+  <si>
+    <t>//*[@id="Flu6humgibSbVSKMGLipUKXy"]</t>
   </si>
 </sst>
 </file>
@@ -535,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -829,4 +851,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: product fields update from pdp
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14C2C1D-0140-4412-B18C-3882C312C2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01378F69-1EF7-4189-87A6-2493BE9A7142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1815" yWindow="840" windowWidth="27000" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24840" yWindow="540" windowWidth="16872" windowHeight="11532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
   <si>
     <t>name</t>
   </si>
@@ -187,16 +187,19 @@
     <t>quantity</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>otCSfuRyXDDgPcWMS82WHWpQ</t>
-  </si>
-  <si>
-    <t>pt-3.5</t>
-  </si>
-  <si>
-    <t>//*[@id="Flu6humgibSbVSKMGLipUKXy"]</t>
+    <t>pt-3</t>
+  </si>
+  <si>
+    <t>tab-content</t>
+  </si>
+  <si>
+    <t>cursor-pointer</t>
+  </si>
+  <si>
+    <t>additional info content</t>
+  </si>
+  <si>
+    <t>additional info click</t>
   </si>
 </sst>
 </file>
@@ -855,15 +858,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -902,15 +905,15 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -918,14 +921,20 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
-      </c>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -940,10 +949,12 @@
       <c r="A13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -960,14 +971,6 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="D21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: introduce method to find and click on available product in PLP page.
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01378F69-1EF7-4189-87A6-2493BE9A7142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504B50B5-A7E7-4702-BA92-EB180C4A653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24840" yWindow="540" windowWidth="16872" windowHeight="11532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
-    <sheet name="PDP_Page" sheetId="2" r:id="rId2"/>
+    <sheet name="Page" sheetId="3" r:id="rId2"/>
+    <sheet name="PDP_Page" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>name</t>
   </si>
@@ -200,13 +201,37 @@
   </si>
   <si>
     <t>additional info click</t>
+  </si>
+  <si>
+    <t>original price</t>
+  </si>
+  <si>
+    <t>//*[@id="pdp-productView"]/div[2]/div[1]/div/div[1]/span[1]</t>
+  </si>
+  <si>
+    <t>sale price</t>
+  </si>
+  <si>
+    <t>//*[@id="pdp-productView"]/div[2]/div[1]/div/div[1]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="pdp-productView"]/div[2]/div[1]/div/div[1]/span</t>
+  </si>
+  <si>
+    <t>price all elements</t>
+  </si>
+  <si>
+    <t>star rating</t>
+  </si>
+  <si>
+    <t>react-rater-star</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +270,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -272,12 +303,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,19 +694,22 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
+      <c r="A8" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>28</v>
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,10 +717,10 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>22</v>
@@ -693,160 +728,146 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
+      <c r="A15" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>31</v>
+      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -857,11 +878,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3895-42F9-4236-940A-C9E9FF890888}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,47 +995,94 @@
         <v>55</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: pdp page complete in current scope, cart page in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504B50B5-A7E7-4702-BA92-EB180C4A653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED824CAF-39AF-4D34-8F15-0EBE23D0E545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="540" windowWidth="16872" windowHeight="11532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24840" yWindow="540" windowWidth="20340" windowHeight="11532" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PLP_Page" sheetId="1" r:id="rId1"/>
-    <sheet name="Page" sheetId="3" r:id="rId2"/>
+    <sheet name="Page" sheetId="3" r:id="rId1"/>
+    <sheet name="PLP_Page" sheetId="1" r:id="rId2"/>
     <sheet name="PDP_Page" sheetId="2" r:id="rId3"/>
+    <sheet name="Cart_Page" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>name</t>
   </si>
@@ -188,6 +189,9 @@
     <t>quantity</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
     <t>pt-3</t>
   </si>
   <si>
@@ -225,6 +229,39 @@
   </si>
   <si>
     <t>react-rater-star</t>
+  </si>
+  <si>
+    <t>add to cart button</t>
+  </si>
+  <si>
+    <t>form-action-addToCart</t>
+  </si>
+  <si>
+    <t>//*[@id="form-action-addToCart"]</t>
+  </si>
+  <si>
+    <t>quantity input</t>
+  </si>
+  <si>
+    <t>//*[@id="qty-c6e9c5ab-f523-482a-b419-57848da66638"]</t>
+  </si>
+  <si>
+    <t>//*[@id="cart-preview-dropdown"]/div/table/tbody/tr/td[2]/div/div[2]/div[1]/input</t>
+  </si>
+  <si>
+    <t>cart preview dropdown</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>to find frame</t>
+  </si>
+  <si>
+    <t>form-input</t>
+  </si>
+  <si>
+    <t>previewCart</t>
   </si>
 </sst>
 </file>
@@ -589,6 +626,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3895-42F9-4236-940A-C9E9FF890888}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -877,56 +959,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3895-42F9-4236-940A-C9E9FF890888}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,80 +1008,96 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
@@ -1083,6 +1137,144 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: cart has all data of added products and displayed products
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED824CAF-39AF-4D34-8F15-0EBE23D0E545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4B92CE-9067-4A99-A3C1-D4E2D6978766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="540" windowWidth="20340" windowHeight="11532" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24840" yWindow="540" windowWidth="20340" windowHeight="11532" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
     <sheet name="PLP_Page" sheetId="1" r:id="rId2"/>
     <sheet name="PDP_Page" sheetId="2" r:id="rId3"/>
     <sheet name="Cart_Page" sheetId="4" r:id="rId4"/>
+    <sheet name="Menu" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>name</t>
   </si>
@@ -262,6 +263,24 @@
   </si>
   <si>
     <t>previewCart</t>
+  </si>
+  <si>
+    <t>previewCartItem</t>
+  </si>
+  <si>
+    <t>drop down products</t>
+  </si>
+  <si>
+    <t>top user cart</t>
+  </si>
+  <si>
+    <t>navUser-item-cartLabel</t>
+  </si>
+  <si>
+    <t>navbar-cart-icon</t>
+  </si>
+  <si>
+    <t>//*[@id="navbar-cart-icon"]</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1176,7 @@
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1225,6 +1244,141 @@
         <v>75</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A0655-15A5-4CC6-9E5D-ABC85E9B1D6D}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>

</xml_diff>

<commit_message>
feat: cart is done, another project add in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4B92CE-9067-4A99-A3C1-D4E2D6978766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845D09B8-6FFC-405F-A41F-3DE25AA1680B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="540" windowWidth="20340" windowHeight="11532" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23808" yWindow="3648" windowWidth="20340" windowHeight="11532" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="86">
   <si>
     <t>name</t>
   </si>
@@ -244,24 +244,21 @@
     <t>quantity input</t>
   </si>
   <si>
-    <t>//*[@id="qty-c6e9c5ab-f523-482a-b419-57848da66638"]</t>
-  </si>
-  <si>
     <t>//*[@id="cart-preview-dropdown"]/div/table/tbody/tr/td[2]/div/div[2]/div[1]/input</t>
   </si>
   <si>
     <t>cart preview dropdown</t>
   </si>
   <si>
+    <t>cart-preview-dropdown</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
     <t>to find frame</t>
   </si>
   <si>
-    <t>form-input</t>
-  </si>
-  <si>
     <t>previewCart</t>
   </si>
   <si>
@@ -281,6 +278,15 @@
   </si>
   <si>
     <t>//*[@id="navbar-cart-icon"]</t>
+  </si>
+  <si>
+    <t>miniCart-qty-update</t>
+  </si>
+  <si>
+    <t>update link elements</t>
+  </si>
+  <si>
+    <t>drop down cart</t>
   </si>
 </sst>
 </file>
@@ -1165,9 +1171,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1210,7 +1216,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1218,42 +1224,48 @@
       <c r="C3" t="s">
         <v>76</v>
       </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
-      </c>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
@@ -1269,9 +1281,11 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
@@ -1291,20 +1305,12 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1316,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A0655-15A5-4CC6-9E5D-ABC85E9B1D6D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,35 +1354,35 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: quick look in progress. complete loading modal window in object
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF40BB9-C5F5-4D58-9E26-BA8CC1C58EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00600121-0881-41E2-AF52-3F7D3701866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24168" yWindow="828" windowWidth="20340" windowHeight="11532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t>name</t>
   </si>
@@ -316,10 +316,22 @@
     <t>modal</t>
   </si>
   <si>
-    <t>quick look popul</t>
-  </si>
-  <si>
     <t>qty[]</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/section[2]/div[1]/div/div[1]/span</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/section[2]/div[1]/div/div[2]/span[2]</t>
+  </si>
+  <si>
+    <t>//*[@id="content1"]/div[1]/p[2]</t>
+  </si>
+  <si>
+    <t>quick look popup</t>
+  </si>
+  <si>
+    <t>sku</t>
   </si>
 </sst>
 </file>
@@ -1030,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,7 +1100,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,126 +1138,156 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>61</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
       <c r="C13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="B16" t="s">
         <v>53</v>
       </c>
       <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: locators for Sign In and new user forms
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00600121-0881-41E2-AF52-3F7D3701866B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02308BC4-8CEB-4B25-B542-F0F3C9890534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="PDP_Page" sheetId="2" r:id="rId3"/>
     <sheet name="Cart_Page" sheetId="4" r:id="rId4"/>
     <sheet name="Menu" sheetId="5" r:id="rId5"/>
+    <sheet name="Sign In" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -332,6 +333,114 @@
   </si>
   <si>
     <t>sku</t>
+  </si>
+  <si>
+    <t>top user sign In</t>
+  </si>
+  <si>
+    <t>/html/body/header/nav/div/ul/li[7]/a/span</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>login_email</t>
+  </si>
+  <si>
+    <t>//*[@id="login_email"]</t>
+  </si>
+  <si>
+    <t>create email</t>
+  </si>
+  <si>
+    <t>create_email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>login_pass</t>
+  </si>
+  <si>
+    <t>//*[@id="login_pass"]</t>
+  </si>
+  <si>
+    <t>sign in button</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[1]/div/div/div[1]/form/div[3]/input</t>
+  </si>
+  <si>
+    <t>forgot password</t>
+  </si>
+  <si>
+    <t>forgot-password</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[1]/div/div/div[1]/form/div[3]/a</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>create_firstName</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>create_lastName</t>
+  </si>
+  <si>
+    <t>//*[@id="create_firstName"]</t>
+  </si>
+  <si>
+    <t>//*[@id="create_lastName"]</t>
+  </si>
+  <si>
+    <t>//*[@id="create_email"]</t>
+  </si>
+  <si>
+    <t>create password</t>
+  </si>
+  <si>
+    <t>create_password</t>
+  </si>
+  <si>
+    <t>//*[@id="create_password"]</t>
+  </si>
+  <si>
+    <t>create_confirmPassword</t>
+  </si>
+  <si>
+    <t>re-enter password</t>
+  </si>
+  <si>
+    <t>//*[@id="create_confirmPassword"]</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>create_phone</t>
+  </si>
+  <si>
+    <t>//*[@id="create_phone"]</t>
+  </si>
+  <si>
+    <t>first order check box</t>
+  </si>
+  <si>
+    <t>checkmark</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[1]/div/div/div[2]/form/label/span</t>
+  </si>
+  <si>
+    <t>create account button</t>
+  </si>
+  <si>
+    <t>/html/body/div[3]/div[1]/div/div/div[2]/form/div[7]/input</t>
   </si>
 </sst>
 </file>
@@ -384,7 +493,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,8 +506,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -406,17 +533,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1044,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1300,7 +1447,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1596,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,6 +1658,17 @@
         <v>82</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
@@ -1566,4 +1724,818 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682C9829-255E-4DD4-AA0C-38B120730660}">
+  <dimension ref="A1:E86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="8"/>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="8"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="8"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="8"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="8"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="8"/>
+      <c r="E80" s="8"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+      <c r="E81" s="8"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: registered user top menu sign in works now
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02308BC4-8CEB-4B25-B542-F0F3C9890534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082570AB-1C18-4FDB-A72D-FE3EC0660CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <t>drop down products</t>
   </si>
   <si>
-    <t>top user cart</t>
-  </si>
-  <si>
     <t>navUser-item-cartLabel</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>sku</t>
   </si>
   <si>
-    <t>top user sign In</t>
-  </si>
-  <si>
     <t>/html/body/header/nav/div/ul/li[7]/a/span</t>
   </si>
   <si>
@@ -441,6 +435,12 @@
   </si>
   <si>
     <t>/html/body/div[3]/div[1]/div/div/div[2]/form/div[7]/input</t>
+  </si>
+  <si>
+    <t>user_sign_in</t>
+  </si>
+  <si>
+    <t>user_cart</t>
   </si>
 </sst>
 </file>
@@ -1172,13 +1172,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1247,7 +1247,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1291,7 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,60 +1362,60 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
         <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
         <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="4"/>
     </row>
@@ -1514,18 +1514,18 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
@@ -1595,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A0655-15A5-4CC6-9E5D-ABC85E9B1D6D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,46 +1627,46 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682C9829-255E-4DD4-AA0C-38B120730660}">
   <dimension ref="A1:E86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,20 +1762,20 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>0</v>
@@ -1788,364 +1788,364 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>105</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>110</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>123</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>

</xml_diff>

<commit_message>
feat: sign in complete, user info complete, shipping address in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082570AB-1C18-4FDB-A72D-FE3EC0660CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85CD1E3-7745-48DA-9804-68F467AE9919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25236" yWindow="528" windowWidth="20340" windowHeight="11532" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="345" windowWidth="20340" windowHeight="11535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Cart_Page" sheetId="4" r:id="rId4"/>
     <sheet name="Menu" sheetId="5" r:id="rId5"/>
     <sheet name="Sign In" sheetId="6" r:id="rId6"/>
+    <sheet name="My_Account_Page" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="152">
   <si>
     <t>name</t>
   </si>
@@ -441,13 +442,58 @@
   </si>
   <si>
     <t>user_cart</t>
+  </si>
+  <si>
+    <t>user_my_account</t>
+  </si>
+  <si>
+    <t>/html/body/header/nav/div/ul/li[7]/a[1]</t>
+  </si>
+  <si>
+    <t>account info</t>
+  </si>
+  <si>
+    <t>AlphaNumericBaseInput</t>
+  </si>
+  <si>
+    <t>account saved text</t>
+  </si>
+  <si>
+    <t>AccountInformation_customSuccess__3Vx0X</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/div/div/div[4]/div[1]/div[1]/div</t>
+  </si>
+  <si>
+    <t>update account button</t>
+  </si>
+  <si>
+    <t>AccountInformationForm_submit__3gY28</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/div/div/div[4]/div[1]/div[1]/form/button</t>
+  </si>
+  <si>
+    <t>Account Info elements</t>
+  </si>
+  <si>
+    <t>Payment elements</t>
+  </si>
+  <si>
+    <t>Shipping elements</t>
+  </si>
+  <si>
+    <t>display elements</t>
+  </si>
+  <si>
+    <t>AddressInfo_container__3Kiim</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,8 +538,59 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,6 +618,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -552,18 +655,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635A0655-15A5-4CC6-9E5D-ABC85E9B1D6D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,6 +1783,17 @@
         <v>100</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
@@ -1731,7 +1856,7 @@
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,796 +1869,968 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="B22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B28" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
+      <c r="A63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
+      <c r="A67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
+      <c r="A69" s="9"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="8"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="8"/>
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
+      <c r="A76" s="9"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="8"/>
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+      <c r="A81" s="9"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="8"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
+      <c r="A84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51C30C4-E94E-49C3-B624-F39C0D0A1DE5}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: shipping address and orders are done
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E85CD1E3-7745-48DA-9804-68F467AE9919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DA34FB-0ACA-4A10-9FF8-AF9DFD40BDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="345" windowWidth="20340" windowHeight="11535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="2145" windowWidth="20340" windowHeight="11535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="158">
   <si>
     <t>name</t>
   </si>
@@ -483,17 +483,35 @@
     <t>Shipping elements</t>
   </si>
   <si>
-    <t>display elements</t>
-  </si>
-  <si>
     <t>AddressInfo_container__3Kiim</t>
+  </si>
+  <si>
+    <t>address info container</t>
+  </si>
+  <si>
+    <t>Shipping_header__3XyRo</t>
+  </si>
+  <si>
+    <t>address headers</t>
+  </si>
+  <si>
+    <t>order table</t>
+  </si>
+  <si>
+    <t>//*[@id="orderHistory"]/table'</t>
+  </si>
+  <si>
+    <t>OrderHistory_orderTable__3pl0l</t>
+  </si>
+  <si>
+    <t>Order Table elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -589,6 +607,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -655,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -678,6 +711,9 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2670,12 +2706,12 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
@@ -2797,40 +2833,63 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>152</v>
+      </c>
       <c r="D12" s="15"/>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="A14" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: shipping address and orders are done, started with test runner
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DA34FB-0ACA-4A10-9FF8-AF9DFD40BDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91A11CB-50DF-45C8-833A-8728FF55C843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2010" yWindow="2145" windowWidth="20340" windowHeight="11535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="158">
   <si>
     <t>name</t>
   </si>
@@ -120,9 +120,6 @@
     <t>collor filters</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
     <t>breadcrumb</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   </si>
   <si>
     <t>Order Table elements</t>
+  </si>
+  <si>
+    <t>fill-current</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -660,6 +660,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -688,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -709,11 +715,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,13 +1032,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:C24"/>
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1163,77 +1172,77 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
+      <c r="A14" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,7 +1256,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,12 +1270,12 @@
         <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
@@ -1280,7 +1289,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -1300,7 +1309,7 @@
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>48</v>
@@ -1308,27 +1317,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1339,10 +1334,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99686DA6-2114-4599-AD6E-A1A7C9CD146A}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,208 +1364,215 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>64</v>
+      <c r="A11" t="s">
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>89</v>
+      <c r="A15" t="s">
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>86</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>91</v>
+      <c r="A17" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1579,12 +1581,16 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1596,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,65 +1629,65 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,7 +1752,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,15 +1778,15 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
@@ -1788,46 +1794,46 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>137</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,7 +1898,7 @@
   <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="A5" sqref="A5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1918,25 +1924,25 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -1949,364 +1955,364 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>107</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>110</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>105</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>125</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>128</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>133</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>134</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -2706,7 +2712,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,12 +2738,12 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -2746,72 +2752,72 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>148</v>
+      <c r="A8" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2824,72 +2830,73 @@
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" s="15"/>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="A13" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="20" t="s">
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: first version of test runner. work in progress for bvt_01
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91A11CB-50DF-45C8-833A-8728FF55C843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EA4F0B-C537-4B1C-A43C-FAB7FAA25D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="2145" windowWidth="20340" windowHeight="11535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2895" yWindow="7215" windowWidth="20340" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
   <si>
     <t>name</t>
   </si>
@@ -505,6 +505,18 @@
   </si>
   <si>
     <t>fill-current</t>
+  </si>
+  <si>
+    <t>on start popup</t>
+  </si>
+  <si>
+    <t>//div[@id="bx-creative-1382906"]</t>
+  </si>
+  <si>
+    <t>close pop up button</t>
+  </si>
+  <si>
+    <t>.//button[@type='reset</t>
   </si>
 </sst>
 </file>
@@ -1003,15 +1015,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3895-42F9-4236-940A-C9E9FF890888}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
   </cols>
@@ -1039,6 +1051,28 @@
       </c>
       <c r="C2" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1050,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,8 +2745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51C30C4-E94E-49C3-B624-F39C0D0A1DE5}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: continue with bvt. store location search is complete
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EA4F0B-C537-4B1C-A43C-FAB7FAA25D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568486D4-E35B-4E77-A666-445B1F360982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="7215" windowWidth="20340" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Menu" sheetId="5" r:id="rId5"/>
     <sheet name="Sign In" sheetId="6" r:id="rId6"/>
     <sheet name="My_Account_Page" sheetId="7" r:id="rId7"/>
+    <sheet name="Store_Location_Page" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="191">
   <si>
     <t>name</t>
   </si>
@@ -517,13 +518,100 @@
   </si>
   <si>
     <t>.//button[@type='reset</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>//*[@id="findInStore"]/div[1]/div[1]/div/div[2]/p[1]</t>
+  </si>
+  <si>
+    <t>//*[@id="findInStore"]/div[1]/div[1]/div/div[2]/p[4]/span[2]</t>
+  </si>
+  <si>
+    <t>zip code</t>
+  </si>
+  <si>
+    <t>findStoreZip</t>
+  </si>
+  <si>
+    <t>//*[@id="findStoreZip"]</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>requestedStoreMiles</t>
+  </si>
+  <si>
+    <t>//*[@id="requestedStoreMiles"]</t>
+  </si>
+  <si>
+    <t>search button</t>
+  </si>
+  <si>
+    <t>//*[@id="findInStoreForm"]/p/div/button</t>
+  </si>
+  <si>
+    <t>select button</t>
+  </si>
+  <si>
+    <t>//*[@id="availableStores"]/li[1]/details/p[2]/button</t>
+  </si>
+  <si>
+    <t>//*[@id="availableStores"]/li[2]/details/p[2]/button</t>
+  </si>
+  <si>
+    <t>storeDetails</t>
+  </si>
+  <si>
+    <t>store found</t>
+  </si>
+  <si>
+    <t>view cart</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/div[2]/section/div/div[2]/a</t>
+  </si>
+  <si>
+    <t>continue shopping</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/div[2]/section/div/div[1]/a</t>
+  </si>
+  <si>
+    <t>//*[@id="modalTitle"]/span</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/button/span/img</t>
+  </si>
+  <si>
+    <t>ql close button</t>
+  </si>
+  <si>
+    <t>search_query</t>
+  </si>
+  <si>
+    <t>//*[@id="search_query"]</t>
+  </si>
+  <si>
+    <t>search input</t>
+  </si>
+  <si>
+    <t>//*[@id="quick-search-form"]/fieldset/div/button/img</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>//*[@id="sort"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,6 +722,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -706,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -735,6 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1015,10 +1111,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2C3895-42F9-4236-940A-C9E9FF890888}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,6 +1171,50 @@
         <v>161</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1082,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,6 +1500,52 @@
         <v>85</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="11"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1371,7 +1557,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C20"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,4 +3121,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AE5261F-F55C-448B-B964-F0134C8A2029}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>177</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add shipping address
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568486D4-E35B-4E77-A666-445B1F360982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9637F5-D3E1-45A7-B880-E907A444E8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="205">
   <si>
     <t>name</t>
   </si>
@@ -605,6 +605,48 @@
   </si>
   <si>
     <t>//*[@id="sort"]</t>
+  </si>
+  <si>
+    <t>swal2-modal</t>
+  </si>
+  <si>
+    <t>no promotion</t>
+  </si>
+  <si>
+    <t>no promotion ok button</t>
+  </si>
+  <si>
+    <t>swal2-confirm</t>
+  </si>
+  <si>
+    <t>checkoutTop-CartPage</t>
+  </si>
+  <si>
+    <t>checkoutBottom-CartPage</t>
+  </si>
+  <si>
+    <t>checkout button top</t>
+  </si>
+  <si>
+    <t>checkout button bottom</t>
+  </si>
+  <si>
+    <t>Shipping_link__300no</t>
+  </si>
+  <si>
+    <t>add change shipping buttons</t>
+  </si>
+  <si>
+    <t>Add New Shipping Address</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>add shipping address button</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/form/button</t>
   </si>
 </sst>
 </file>
@@ -801,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -831,6 +873,9 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,7 +1159,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1823,12 +1868,12 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
@@ -1911,19 +1956,48 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
@@ -2929,18 +3003,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51C30C4-E94E-49C3-B624-F39C0D0A1DE5}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3084,39 +3158,82 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>155</v>
-      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: cart work mostly
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9637F5-D3E1-45A7-B880-E907A444E8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6F1840-ED84-4279-A310-1020584DD531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="285" windowWidth="26205" windowHeight="14235" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="225">
   <si>
     <t>name</t>
   </si>
@@ -244,9 +244,6 @@
     <t>quantity input</t>
   </si>
   <si>
-    <t>//*[@id="cart-preview-dropdown"]/div/table/tbody/tr/td[2]/div/div[2]/div[1]/input</t>
-  </si>
-  <si>
     <t>cart preview dropdown</t>
   </si>
   <si>
@@ -619,6 +616,9 @@
     <t>swal2-confirm</t>
   </si>
   <si>
+    <t>checkout button</t>
+  </si>
+  <si>
     <t>checkoutTop-CartPage</t>
   </si>
   <si>
@@ -640,13 +640,73 @@
     <t>Add New Shipping Address</t>
   </si>
   <si>
-    <t>ad</t>
-  </si>
-  <si>
     <t>add shipping address button</t>
   </si>
   <si>
     <t>//*[@id="modal"]/div[1]/div/form/button</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/form/button/div</t>
+  </si>
+  <si>
+    <t>add change address buttons</t>
+  </si>
+  <si>
+    <t>use this address button</t>
+  </si>
+  <si>
+    <t>//*[@id="modal"]/div[1]/div/div/p[6]/button[1]</t>
+  </si>
+  <si>
+    <t>ignore button</t>
+  </si>
+  <si>
+    <t>close new address button</t>
+  </si>
+  <si>
+    <t>viewCart-Cmodal</t>
+  </si>
+  <si>
+    <t>//*[@id="viewCart-CModal"]</t>
+  </si>
+  <si>
+    <t>view cart button</t>
+  </si>
+  <si>
+    <t>checkout-Cmodal</t>
+  </si>
+  <si>
+    <t>update buttons</t>
+  </si>
+  <si>
+    <t>cart-item-update</t>
+  </si>
+  <si>
+    <t>delete buttons</t>
+  </si>
+  <si>
+    <t>previewCartItem-remove</t>
+  </si>
+  <si>
+    <t>form-input.form-input--incrementTotal</t>
+  </si>
+  <si>
+    <t>cart total</t>
+  </si>
+  <si>
+    <t>//*[@id="total-savings"]/div[2]/span</t>
+  </si>
+  <si>
+    <t>//*[@id="cart-preview-dropdown"]/div/div[2]/div[2]/div[1]/div[2]/span</t>
+  </si>
+  <si>
+    <t>cart total savings</t>
+  </si>
+  <si>
+    <t>item subtotals</t>
+  </si>
+  <si>
+    <t>previewCartItem-subtotal</t>
   </si>
 </sst>
 </file>
@@ -1196,68 +1256,68 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>158</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>160</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1330,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,59 +1596,59 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B22" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1657,7 +1717,7 @@
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1690,7 +1750,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1712,7 +1772,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,7 +1794,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1783,60 +1843,60 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
         <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" s="4"/>
     </row>
@@ -1865,10 +1925,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,7 +1954,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,79 +1962,79 @@
         <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1999,41 +2059,104 @@
         <v>196</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>210</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>213</v>
+      </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>220</v>
+      </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>221</v>
+      </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2046,7 +2169,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,62 +2195,62 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,25 +2341,25 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>0</v>
@@ -2249,364 +2372,364 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>132</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
@@ -3003,10 +3126,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51C30C4-E94E-49C3-B624-F39C0D0A1DE5}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,12 +3155,12 @@
         <v>7</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -3046,72 +3169,72 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -3125,7 +3248,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -3134,105 +3257,150 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="15"/>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D13" s="15"/>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="17" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C22" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3245,7 +3413,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,13 +3440,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>162</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,139 +3457,139 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>171</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>173</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>178</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>180</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: checkout in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61A8C3B5-F9DF-4855-B876-F43D27B8866F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83590392-9416-42E4-8EBC-1E121C52A5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="285" windowWidth="26205" windowHeight="14235" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sign In" sheetId="6" r:id="rId6"/>
     <sheet name="My_Account_Page" sheetId="7" r:id="rId7"/>
     <sheet name="Store_Location_Page" sheetId="8" r:id="rId8"/>
+    <sheet name="Checkout_Page" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="262">
   <si>
     <t>name</t>
   </si>
@@ -722,13 +723,109 @@
   </si>
   <si>
     <t>cart-item-block.cart-item-title</t>
+  </si>
+  <si>
+    <t>apply promo button</t>
+  </si>
+  <si>
+    <t>couponcode</t>
+  </si>
+  <si>
+    <t>//*[@id="couponcode"]</t>
+  </si>
+  <si>
+    <t>openPromoCode-CartPage</t>
+  </si>
+  <si>
+    <t>coupon-code-add</t>
+  </si>
+  <si>
+    <t>//*[@id="openPromoCode-CartPage"]</t>
+  </si>
+  <si>
+    <t>open promo code</t>
+  </si>
+  <si>
+    <t>promo code input</t>
+  </si>
+  <si>
+    <t>applyPromoCode-CartPage</t>
+  </si>
+  <si>
+    <t>//*[@id="applyPromoCode-CartPage"]</t>
+  </si>
+  <si>
+    <t>apply promo error modal</t>
+  </si>
+  <si>
+    <t>promo error ok button</t>
+  </si>
+  <si>
+    <t>swal2-confirm.button</t>
+  </si>
+  <si>
+    <t>swal2-modal.swal2-show</t>
+  </si>
+  <si>
+    <t>//*[@id="checkoutTop-CartPage"]</t>
+  </si>
+  <si>
+    <t>//*[@id="checkoutBottom-CartPage"]</t>
+  </si>
+  <si>
+    <t>guest email</t>
+  </si>
+  <si>
+    <t>checkoutV2</t>
+  </si>
+  <si>
+    <t>//*[@id='checkoutV2']</t>
+  </si>
+  <si>
+    <t>checkout iframe</t>
+  </si>
+  <si>
+    <t>guestCheckoutEmail</t>
+  </si>
+  <si>
+    <t>//*[@id="guestCheckoutEmail"]</t>
+  </si>
+  <si>
+    <t>guest checkout button</t>
+  </si>
+  <si>
+    <t>loginModal-guestCheckout</t>
+  </si>
+  <si>
+    <t>//*[@id="loginModal-guestCheckout"]</t>
+  </si>
+  <si>
+    <t>ql product info</t>
+  </si>
+  <si>
+    <t>content1</t>
+  </si>
+  <si>
+    <t>//*[@id="content1"]</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Guest Login</t>
+  </si>
+  <si>
+    <t>shippingAddress-firstName</t>
+  </si>
+  <si>
+    <t>//*[@id="shippingAddress-firstName"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,8 +943,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -890,6 +1008,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -918,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -951,6 +1075,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1677,7 +1807,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,11 +2046,27 @@
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>256</v>
+      </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,6 +2079,7 @@
       <c r="A25" s="5"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1940,10 +2087,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F6E225-3942-4B5C-A70E-AF2C84CA4C46}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,157 +2223,286 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="B14" t="s">
         <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>213</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>210</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
-      </c>
-      <c r="D15" s="4"/>
+        <v>211</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>224</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>228</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3483,7 +3759,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3702,4 +3978,196 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725FA841-A7E4-45E2-8814-AD642CB9BF88}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>251</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: paypal payment done.
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B3F8F9-5DE4-4E15-A7D7-FDC2197A2C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0406300-92EF-4408-B398-0CC5C3C2FDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="0" windowWidth="26880" windowHeight="13200" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="282">
   <si>
     <t>name</t>
   </si>
@@ -844,6 +844,42 @@
   </si>
   <si>
     <t>checkout with paypal buttons</t>
+  </si>
+  <si>
+    <t>paypal email input</t>
+  </si>
+  <si>
+    <t>paypal next button</t>
+  </si>
+  <si>
+    <t>btnNext</t>
+  </si>
+  <si>
+    <t>paypal password</t>
+  </si>
+  <si>
+    <t>login-password</t>
+  </si>
+  <si>
+    <t>paypal login button</t>
+  </si>
+  <si>
+    <t>btnLogin</t>
+  </si>
+  <si>
+    <t>payment-submit-btn</t>
+  </si>
+  <si>
+    <t>//*[@id="payment-submit-btn"]</t>
+  </si>
+  <si>
+    <t>paypal pay now button</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/div/div[2]/div[2]/div[2]/div[1]/div/div/span</t>
+  </si>
+  <si>
+    <t>order number</t>
   </si>
 </sst>
 </file>
@@ -1497,10 +1533,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60470D90-63EA-42CC-9FC2-78A65FF8DD8C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1553,10 +1589,114 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>278</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4076,10 +4216,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725FA841-A7E4-45E2-8814-AD642CB9BF88}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:C15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,11 +4397,16 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="4"/>
-    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>280</v>
+      </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4274,12 +4419,16 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: paypal payment done. order validation in progress
</commit_message>
<xml_diff>
--- a/test_data/locators.xlsx
+++ b/test_data/locators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0406300-92EF-4408-B398-0CC5C3C2FDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEBC51A-EF7A-4527-B14E-873078A44933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="0" windowWidth="26880" windowHeight="13200" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="3555" windowWidth="26880" windowHeight="13200" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="288">
   <si>
     <t>name</t>
   </si>
@@ -880,6 +880,24 @@
   </si>
   <si>
     <t>order number</t>
+  </si>
+  <si>
+    <t>order iframe</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/iframe</t>
+  </si>
+  <si>
+    <t>billing address</t>
+  </si>
+  <si>
+    <t>After purchase page</t>
+  </si>
+  <si>
+    <t>//*[@id="__next"]/div/div[2]/div[2]/div[3]/div[1]/div</t>
+  </si>
+  <si>
+    <t>AddressSummary_addressContainer__2K64l</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1044,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1075,6 +1093,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1103,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1142,6 +1166,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,7 +1560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60470D90-63EA-42CC-9FC2-78A65FF8DD8C}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4216,10 +4241,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725FA841-A7E4-45E2-8814-AD642CB9BF88}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4285,13 +4310,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>250</v>
+        <v>283</v>
       </c>
       <c r="D5" s="27"/>
       <c r="E5" s="27"/>
@@ -4301,23 +4326,23 @@
         <v>246</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="27"/>
@@ -4327,28 +4352,30 @@
         <v>252</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D8" s="27"/>
       <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4356,79 +4383,121 @@
         <v>112</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>262</v>
+        <v>112</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>138</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>264</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>263</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="C14" s="27" t="s">
+        <v>264</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="B16" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="27" t="s">
+      <c r="B18" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>286</v>
+      </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>